<commit_message>
New design and CI colors
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -22,7 +22,7 @@
     <t>Author: Lauritz Holtmann</t>
   </si>
   <si>
-    <t>Date: 2023-04-03</t>
+    <t>Date: 2025-09-09</t>
   </si>
   <si>
     <t>Finding-ID</t>
@@ -37,7 +37,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>#PEN20230001</t>
+    <t>#PEN20250001</t>
   </si>
   <si>
     <t>Critical (9.1)</t>
@@ -49,7 +49,7 @@
     <t>XXE in Test Shop</t>
   </si>
   <si>
-    <t>#PEN20230002</t>
+    <t>#PEN20250002</t>
   </si>
   <si>
     <t>High (7.1)</t>
@@ -58,7 +58,7 @@
     <t>XSS in Test Shop</t>
   </si>
   <si>
-    <t>#PEN20230003</t>
+    <t>#PEN20250003</t>
   </si>
   <si>
     <t>Low (3.1)</t>

</xml_diff>

<commit_message>
feat: Add handling of fixed vulnerabilities and improve Excel output
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Pentest Report: Example Report</t>
   </si>
@@ -22,12 +22,15 @@
     <t>Author: Lauritz Holtmann</t>
   </si>
   <si>
-    <t>Date: 2025-09-09</t>
+    <t>Date: 2025-09-25</t>
   </si>
   <si>
     <t>Finding-ID</t>
   </si>
   <si>
+    <t>Fixed</t>
+  </si>
+  <si>
     <t>Severity</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>#PEN20250001</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Critical (9.1)</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
   </si>
   <si>
     <t>#PEN20250002</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>High (7.1)</t>
@@ -71,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +96,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +122,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC8C8CF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC62828"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7B1FA2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E7D32"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD32F2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF59D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,10 +168,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,28 +475,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -446,47 +515,59 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Visual Redesign (use matching colors for listings), coherently handle finding_ids and fixed findings
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -22,7 +22,7 @@
     <t>Author: Lauritz Holtmann</t>
   </si>
   <si>
-    <t>Date: 2025-09-25</t>
+    <t>Date: 2025-11-18</t>
   </si>
   <si>
     <t>Finding-ID</t>
@@ -67,7 +67,7 @@
     <t>XSS in Test Shop</t>
   </si>
   <si>
-    <t>#PEN20250003</t>
+    <t>#PEN-TEST-0003</t>
   </si>
   <si>
     <t>Low (3.1)</t>

</xml_diff>

<commit_message>
Update from CVSS3.1 to CVSS4.0
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -46,7 +46,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Critical (9.1)</t>
+    <t>Critical (9.3)</t>
   </si>
   <si>
     <t>Test Shop</t>
@@ -61,16 +61,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>High (7.1)</t>
+    <t>High (7.0)</t>
   </si>
   <si>
     <t>XSS in Test Shop</t>
   </si>
   <si>
-    <t>#PEN-TEST-0003</t>
-  </si>
-  <si>
-    <t>Low (3.1)</t>
+    <t>#PEN20250003</t>
+  </si>
+  <si>
+    <t>Medium (5.6)</t>
   </si>
   <si>
     <t>Open Redirect in Test Shop</t>
@@ -105,6 +105,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -151,7 +152,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF59D"/>
+        <fgColor rgb="FFF9A825"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>

<commit_message>
Improve Excel export, introduce optional comment
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Pentest Report: Example Report</t>
   </si>
@@ -40,6 +40,12 @@
     <t>Title</t>
   </si>
   <si>
+    <t>CVSS v4.0 Vector</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>#PEN20250001</t>
   </si>
   <si>
@@ -55,6 +61,12 @@
     <t>XXE in Test Shop</t>
   </si>
   <si>
+    <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:N/VC:H/VI:H/VA:N/SC:N/SI:N/SA:N</t>
+  </si>
+  <si>
+    <t>The API processes external entities that are included within the request body.</t>
+  </si>
+  <si>
     <t>#PEN20250002</t>
   </si>
   <si>
@@ -67,6 +79,12 @@
     <t>XSS in Test Shop</t>
   </si>
   <si>
+    <t>CVSS:4.0/AV:N/AC:L/AT:N/PR:N/UI:A/VC:H/VI:L/VA:N/SC:N/SI:N/SA:N</t>
+  </si>
+  <si>
+    <t>The xyz parameter is not correctly encoded and/or filtered before being embedded within the application.</t>
+  </si>
+  <si>
     <t>#PEN20250003</t>
   </si>
   <si>
@@ -74,6 +92,12 @@
   </si>
   <si>
     <t>Open Redirect in Test Shop</t>
+  </si>
+  <si>
+    <t>CVSS:4.0/AV:N/AC:H/AT:P/PR:H/UI:A/VC:H/VI:N/VA:N/SC:N/SI:N/SA:N</t>
+  </si>
+  <si>
+    <t>The to parameter is used to redirect the end-user without sufficient validation.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,25 +509,27 @@
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -519,56 +545,80 @@
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>